<commit_message>
support single sentence query
</commit_message>
<xml_diff>
--- a/data for mat.xlsx
+++ b/data for mat.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20910"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16440" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16600" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="raw L" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Feature" sheetId="3" r:id="rId3"/>
     <sheet name="indep L" sheetId="5" r:id="rId4"/>
     <sheet name="depend L" sheetId="4" r:id="rId5"/>
+    <sheet name="工作表2" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1679" uniqueCount="766">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1684" uniqueCount="771">
   <si>
     <t>1.4.1</t>
   </si>
@@ -2393,6 +2394,26 @@
     <t>sum_feature</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>7.12.11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7.12.13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7.12.15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7.12.17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7.12.19</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -2520,8 +2541,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2555,16 +2578,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="11">
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -2865,7 +2890,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P170"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
+    <sheetView topLeftCell="A42" workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
@@ -44521,8 +44546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI269"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="M105" sqref="M105"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="N96" sqref="N96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -72198,8 +72223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="D68" sqref="D68"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -73354,7 +73379,7 @@
         <v>703</v>
       </c>
       <c r="B33">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C33" s="2">
         <f>'raw L'!C33/'indep L &amp; F'!$B33</f>
@@ -73390,7 +73415,7 @@
         <v>704</v>
       </c>
       <c r="B34">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C34" s="2">
         <f>'raw L'!C34/'indep L &amp; F'!$B34</f>
@@ -73462,7 +73487,7 @@
         <v>705</v>
       </c>
       <c r="B36">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C36" s="2">
         <f>'raw L'!C36/'indep L &amp; F'!$B36</f>
@@ -73534,7 +73559,7 @@
         <v>708</v>
       </c>
       <c r="B38">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C38" s="2">
         <f>'raw L'!C38/'indep L &amp; F'!$B38</f>
@@ -73570,7 +73595,7 @@
         <v>709</v>
       </c>
       <c r="B39">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C39" s="2">
         <f>'raw L'!C39/'indep L &amp; F'!$B39</f>
@@ -73678,7 +73703,7 @@
         <v>711</v>
       </c>
       <c r="B42">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C42" s="2">
         <f>'raw L'!C42/'indep L &amp; F'!$B42</f>
@@ -73750,7 +73775,7 @@
         <v>712</v>
       </c>
       <c r="B44">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C44" s="2">
         <f>'raw L'!C44/'indep L &amp; F'!$B44</f>
@@ -74146,7 +74171,7 @@
         <v>718</v>
       </c>
       <c r="B55">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C55" s="2">
         <f>'raw L'!C55/'indep L &amp; F'!$B55</f>
@@ -74254,7 +74279,7 @@
         <v>720</v>
       </c>
       <c r="B58">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C58" s="2">
         <f>'raw L'!C58/'indep L &amp; F'!$B58</f>
@@ -74538,9 +74563,11 @@
       </c>
     </row>
     <row r="66" spans="1:9">
-      <c r="A66" s="13"/>
+      <c r="A66" s="13" t="s">
+        <v>766</v>
+      </c>
       <c r="B66" s="13">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C66" s="2">
         <f>'raw L'!C66/'indep L &amp; F'!$B66</f>
@@ -74608,8 +74635,11 @@
       </c>
     </row>
     <row r="68" spans="1:9">
+      <c r="A68" s="13" t="s">
+        <v>767</v>
+      </c>
       <c r="B68">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C68" s="2">
         <f>'raw L'!C68/'indep L &amp; F'!$B68</f>
@@ -74677,8 +74707,11 @@
       </c>
     </row>
     <row r="70" spans="1:9">
+      <c r="A70" t="s">
+        <v>768</v>
+      </c>
       <c r="B70">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C70" s="2">
         <f>'raw L'!C70/'indep L &amp; F'!$B70</f>
@@ -74746,8 +74779,11 @@
       </c>
     </row>
     <row r="72" spans="1:9">
+      <c r="A72" t="s">
+        <v>769</v>
+      </c>
       <c r="B72">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C72" s="2">
         <f>'raw L'!C72/'indep L &amp; F'!$B72</f>
@@ -74815,8 +74851,11 @@
       </c>
     </row>
     <row r="74" spans="1:9">
+      <c r="A74" t="s">
+        <v>770</v>
+      </c>
       <c r="B74">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C74" s="2">
         <f>'raw L'!C74/'indep L &amp; F'!$B74</f>
@@ -75284,7 +75323,7 @@
         <v>733</v>
       </c>
       <c r="B87">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C87" s="2">
         <f>'raw L'!C87/'indep L &amp; F'!$B87</f>
@@ -75320,7 +75359,7 @@
         <v>734</v>
       </c>
       <c r="B88">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C88" s="2">
         <f>'raw L'!C88/'indep L &amp; F'!$B88</f>
@@ -75356,7 +75395,7 @@
         <v>735</v>
       </c>
       <c r="B89">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C89" s="2">
         <f>'raw L'!C89/'indep L &amp; F'!$B89</f>
@@ -75392,7 +75431,7 @@
         <v>736</v>
       </c>
       <c r="B90">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C90" s="2">
         <f>'raw L'!C90/'indep L &amp; F'!$B90</f>
@@ -75536,7 +75575,7 @@
         <v>739</v>
       </c>
       <c r="B94">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C94" s="2">
         <f>'raw L'!C94/'indep L &amp; F'!$B94</f>
@@ -75932,7 +75971,7 @@
         <v>742</v>
       </c>
       <c r="B105">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C105" s="2">
         <f>'raw L'!C105/'indep L &amp; F'!$B105</f>
@@ -76112,7 +76151,7 @@
         <v>743</v>
       </c>
       <c r="B110">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C110" s="2">
         <f>'raw L'!C110/'indep L &amp; F'!$B110</f>
@@ -76148,7 +76187,7 @@
         <v>744</v>
       </c>
       <c r="B111">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C111" s="2">
         <f>'raw L'!C111/'indep L &amp; F'!$B111</f>
@@ -76184,7 +76223,7 @@
         <v>745</v>
       </c>
       <c r="B112">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C112" s="2">
         <f>'raw L'!C112/'indep L &amp; F'!$B112</f>
@@ -76220,7 +76259,7 @@
         <v>746</v>
       </c>
       <c r="B113">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C113" s="2">
         <f>'raw L'!C113/'indep L &amp; F'!$B113</f>
@@ -76292,7 +76331,7 @@
         <v>747</v>
       </c>
       <c r="B115">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C115" s="2">
         <f>'raw L'!C115/'indep L &amp; F'!$B115</f>
@@ -76328,7 +76367,7 @@
         <v>748</v>
       </c>
       <c r="B116">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C116" s="2">
         <f>'raw L'!C116/'indep L &amp; F'!$B116</f>
@@ -76364,7 +76403,7 @@
         <v>749</v>
       </c>
       <c r="B117">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C117" s="2">
         <f>'raw L'!C117/'indep L &amp; F'!$B117</f>
@@ -76472,7 +76511,7 @@
         <v>750</v>
       </c>
       <c r="B120">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C120" s="2">
         <f>'raw L'!C120/'indep L &amp; F'!$B120</f>
@@ -76616,7 +76655,7 @@
         <v>751</v>
       </c>
       <c r="B124">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C124" s="2">
         <f>'raw L'!C124/'indep L &amp; F'!$B124</f>
@@ -76652,7 +76691,7 @@
         <v>752</v>
       </c>
       <c r="B125">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C125" s="2">
         <f>'raw L'!C125/'indep L &amp; F'!$B125</f>
@@ -76688,7 +76727,7 @@
         <v>753</v>
       </c>
       <c r="B126">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C126" s="2">
         <f>'raw L'!C126/'indep L &amp; F'!$B126</f>
@@ -76724,7 +76763,7 @@
         <v>754</v>
       </c>
       <c r="B127">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C127" s="2">
         <f>'raw L'!C127/'indep L &amp; F'!$B127</f>
@@ -76796,7 +76835,7 @@
         <v>755</v>
       </c>
       <c r="B129">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C129" s="2">
         <f>'raw L'!C129/'indep L &amp; F'!$B129</f>
@@ -76868,7 +76907,7 @@
         <v>756</v>
       </c>
       <c r="B131">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C131" s="2">
         <f>'raw L'!C131/'indep L &amp; F'!$B131</f>
@@ -76904,7 +76943,7 @@
         <v>757</v>
       </c>
       <c r="B132">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C132" s="2">
         <f>'raw L'!C132/'indep L &amp; F'!$B132</f>
@@ -76976,7 +77015,7 @@
         <v>758</v>
       </c>
       <c r="B134">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C134" s="2">
         <f>'raw L'!C134/'indep L &amp; F'!$B134</f>
@@ -77012,7 +77051,7 @@
         <v>759</v>
       </c>
       <c r="B135">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C135" s="2">
         <f>'raw L'!C135/'indep L &amp; F'!$B135</f>
@@ -77228,7 +77267,7 @@
         <v>406</v>
       </c>
       <c r="B141">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C141" s="2">
         <f>'raw L'!C141/'indep L &amp; F'!$B141</f>
@@ -77264,7 +77303,7 @@
         <v>409</v>
       </c>
       <c r="B142">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C142" s="2">
         <f>'raw L'!C142/'indep L &amp; F'!$B142</f>
@@ -77300,7 +77339,7 @@
         <v>411</v>
       </c>
       <c r="B143">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C143" s="2">
         <f>'raw L'!C143/'indep L &amp; F'!$B143</f>
@@ -77336,7 +77375,7 @@
         <v>413</v>
       </c>
       <c r="B144">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C144" s="2">
         <f>'raw L'!C144/'indep L &amp; F'!$B144</f>
@@ -77372,7 +77411,7 @@
         <v>415</v>
       </c>
       <c r="B145">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C145" s="2">
         <f>'raw L'!C145/'indep L &amp; F'!$B145</f>
@@ -77408,7 +77447,7 @@
         <v>417</v>
       </c>
       <c r="B146">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C146" s="2">
         <f>'raw L'!C146/'indep L &amp; F'!$B146</f>
@@ -77444,7 +77483,7 @@
         <v>419</v>
       </c>
       <c r="B147">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C147" s="2">
         <f>'raw L'!C147/'indep L &amp; F'!$B147</f>
@@ -77516,7 +77555,7 @@
         <v>423</v>
       </c>
       <c r="B149">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C149" s="2">
         <f>'raw L'!C149/'indep L &amp; F'!$B149</f>
@@ -77552,7 +77591,7 @@
         <v>425</v>
       </c>
       <c r="B150">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C150" s="2">
         <f>'raw L'!C150/'indep L &amp; F'!$B150</f>
@@ -77588,7 +77627,7 @@
         <v>427</v>
       </c>
       <c r="B151">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C151" s="2">
         <f>'raw L'!C151/'indep L &amp; F'!$B151</f>
@@ -77624,7 +77663,7 @@
         <v>429</v>
       </c>
       <c r="B152">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C152" s="2">
         <f>'raw L'!C152/'indep L &amp; F'!$B152</f>
@@ -77660,7 +77699,7 @@
         <v>760</v>
       </c>
       <c r="B153">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C153" s="2">
         <f>'raw L'!C153/'indep L &amp; F'!$B153</f>
@@ -77696,7 +77735,7 @@
         <v>761</v>
       </c>
       <c r="B154">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C154" s="2">
         <f>'raw L'!C154/'indep L &amp; F'!$B154</f>
@@ -77768,7 +77807,7 @@
         <v>437</v>
       </c>
       <c r="B156">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C156" s="2">
         <f>'raw L'!C156/'indep L &amp; F'!$B156</f>
@@ -77804,7 +77843,7 @@
         <v>439</v>
       </c>
       <c r="B157">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C157" s="2">
         <f>'raw L'!C157/'indep L &amp; F'!$B157</f>
@@ -77840,7 +77879,7 @@
         <v>441</v>
       </c>
       <c r="B158">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C158" s="2">
         <f>'raw L'!C158/'indep L &amp; F'!$B158</f>
@@ -77876,7 +77915,7 @@
         <v>443</v>
       </c>
       <c r="B159">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C159" s="2">
         <f>'raw L'!C159/'indep L &amp; F'!$B159</f>
@@ -77912,7 +77951,7 @@
         <v>445</v>
       </c>
       <c r="B160">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C160" s="2">
         <f>'raw L'!C160/'indep L &amp; F'!$B160</f>
@@ -77984,7 +78023,7 @@
         <v>762</v>
       </c>
       <c r="B162">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C162" s="2">
         <f>'raw L'!C162/'indep L &amp; F'!$B162</f>
@@ -78068,7 +78107,7 @@
   <dimension ref="A1:AZ269"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -95145,4 +95184,24 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>